<commit_message>
Polish Jinja2 Template Render
</commit_message>
<xml_diff>
--- a/app/algorithm/database/data.xlsx
+++ b/app/algorithm/database/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\IAI\app\algorithm\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36319A26-1EC5-4529-ADC7-635D4D0C4DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BA635A-59A4-47B1-A31C-A8C70716E9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="708" yWindow="24" windowWidth="11796" windowHeight="11880" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Train" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1672,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF04A2D-250E-4B16-8195-1DA5D0BCE093}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+    <sheetView topLeftCell="A235" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -5030,4 +5031,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4479DC75-C441-46FF-B23E-A1E53BC389B8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test google map API
</commit_message>
<xml_diff>
--- a/app/algorithm/database/data.xlsx
+++ b/app/algorithm/database/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\IAI\app\algorithm\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6403342-6238-4139-B730-63FA3DC6084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FA5CAF-921B-4D00-A9C3-BC342B9A651E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="520">
   <si>
     <t>message</t>
   </si>
@@ -1588,6 +1588,12 @@
   </si>
   <si>
     <t>Name me some accommodations with good service</t>
+  </si>
+  <si>
+    <t>Please recommend me some hostel</t>
+  </si>
+  <si>
+    <t>Accomodations</t>
   </si>
 </sst>
 </file>
@@ -1952,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF04A2D-250E-4B16-8195-1DA5D0BCE093}">
-  <dimension ref="A1:B514"/>
+  <dimension ref="A1:B516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,7 +2036,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B9" t="s">
         <v>492</v>
@@ -2038,7 +2044,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="B10" t="s">
         <v>492</v>
@@ -2046,7 +2052,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B11" t="s">
         <v>492</v>
@@ -2054,7 +2060,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B12" t="s">
         <v>492</v>
@@ -2062,7 +2068,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B13" t="s">
         <v>492</v>
@@ -2070,7 +2076,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B14" t="s">
         <v>492</v>
@@ -2078,7 +2084,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B15" t="s">
         <v>492</v>
@@ -2086,7 +2092,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B16" t="s">
         <v>492</v>
@@ -2094,7 +2100,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B17" t="s">
         <v>492</v>
@@ -2102,7 +2108,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B18" t="s">
         <v>492</v>
@@ -2110,7 +2116,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B19" t="s">
         <v>492</v>
@@ -2118,7 +2124,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>491</v>
+        <v>516</v>
       </c>
       <c r="B20" t="s">
         <v>492</v>
@@ -2126,7 +2132,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>493</v>
+        <v>517</v>
       </c>
       <c r="B21" t="s">
         <v>492</v>
@@ -2134,7 +2140,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B22" t="s">
         <v>492</v>
@@ -2142,7 +2148,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B23" t="s">
         <v>492</v>
@@ -2150,7 +2156,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B24" t="s">
         <v>492</v>
@@ -2158,7 +2164,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B25" t="s">
         <v>492</v>
@@ -2166,7 +2172,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B26" t="s">
         <v>492</v>
@@ -2174,7 +2180,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B27" t="s">
         <v>492</v>
@@ -2182,23 +2188,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>273</v>
+        <v>498</v>
       </c>
       <c r="B28" t="s">
-        <v>274</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>275</v>
+        <v>499</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B30" t="s">
         <v>274</v>
@@ -2206,7 +2212,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B31" t="s">
         <v>274</v>
@@ -2214,7 +2220,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B32" t="s">
         <v>274</v>
@@ -2222,7 +2228,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B33" t="s">
         <v>274</v>
@@ -2230,7 +2236,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B34" t="s">
         <v>274</v>
@@ -2238,7 +2244,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B35" t="s">
         <v>274</v>
@@ -2246,7 +2252,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B36" t="s">
         <v>274</v>
@@ -2254,7 +2260,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B37" t="s">
         <v>274</v>
@@ -2262,7 +2268,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B38" t="s">
         <v>274</v>
@@ -2270,7 +2276,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B39" t="s">
         <v>274</v>
@@ -2278,7 +2284,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B40" t="s">
         <v>274</v>
@@ -2286,7 +2292,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B41" t="s">
         <v>274</v>
@@ -2294,7 +2300,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B42" t="s">
         <v>274</v>
@@ -2302,7 +2308,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s">
         <v>274</v>
@@ -2310,7 +2316,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s">
         <v>274</v>
@@ -2318,7 +2324,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B45" t="s">
         <v>274</v>
@@ -2326,7 +2332,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s">
         <v>274</v>
@@ -2334,7 +2340,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B47" t="s">
         <v>274</v>
@@ -2342,7 +2348,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B48" t="s">
         <v>274</v>
@@ -2350,7 +2356,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B49" t="s">
         <v>274</v>
@@ -2358,7 +2364,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B50" t="s">
         <v>274</v>
@@ -2366,7 +2372,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B51" t="s">
         <v>274</v>
@@ -2374,7 +2380,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B52" t="s">
         <v>274</v>
@@ -2382,7 +2388,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B53" t="s">
         <v>274</v>
@@ -2390,7 +2396,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B54" t="s">
         <v>274</v>
@@ -2398,7 +2404,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B55" t="s">
         <v>274</v>
@@ -2406,7 +2412,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B56" t="s">
         <v>274</v>
@@ -2414,7 +2420,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B57" t="s">
         <v>274</v>
@@ -2422,7 +2428,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B58" t="s">
         <v>274</v>
@@ -2430,7 +2436,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B59" t="s">
         <v>274</v>
@@ -2438,7 +2444,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B60" t="s">
         <v>274</v>
@@ -2446,7 +2452,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B61" t="s">
         <v>274</v>
@@ -2454,7 +2460,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B62" t="s">
         <v>274</v>
@@ -2462,7 +2468,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B63" t="s">
         <v>274</v>
@@ -2470,7 +2476,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B64" t="s">
         <v>274</v>
@@ -2478,7 +2484,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B65" t="s">
         <v>274</v>
@@ -2486,7 +2492,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>396</v>
+        <v>310</v>
       </c>
       <c r="B66" t="s">
         <v>274</v>
@@ -2494,7 +2500,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>397</v>
+        <v>311</v>
       </c>
       <c r="B67" t="s">
         <v>274</v>
@@ -2502,7 +2508,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B68" t="s">
         <v>274</v>
@@ -2510,7 +2516,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B69" t="s">
         <v>274</v>
@@ -2518,7 +2524,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B70" t="s">
         <v>274</v>
@@ -2526,7 +2532,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B71" t="s">
         <v>274</v>
@@ -2534,7 +2540,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B72" t="s">
         <v>274</v>
@@ -2542,7 +2548,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B73" t="s">
         <v>274</v>
@@ -2550,7 +2556,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B74" t="s">
         <v>274</v>
@@ -2558,7 +2564,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B75" t="s">
         <v>274</v>
@@ -2566,7 +2572,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B76" t="s">
         <v>274</v>
@@ -2574,7 +2580,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B77" t="s">
         <v>274</v>
@@ -2582,7 +2588,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B78" t="s">
         <v>274</v>
@@ -2590,7 +2596,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B79" t="s">
         <v>274</v>
@@ -2598,7 +2604,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B80" t="s">
         <v>274</v>
@@ -2606,7 +2612,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>484</v>
+        <v>409</v>
       </c>
       <c r="B81" t="s">
         <v>274</v>
@@ -2614,7 +2620,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>485</v>
+        <v>410</v>
       </c>
       <c r="B82" t="s">
         <v>274</v>
@@ -2622,7 +2628,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B83" t="s">
         <v>274</v>
@@ -2630,7 +2636,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B84" t="s">
         <v>274</v>
@@ -2638,7 +2644,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>309</v>
+        <v>486</v>
       </c>
       <c r="B85" t="s">
         <v>274</v>
@@ -2646,7 +2652,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B86" t="s">
         <v>274</v>
@@ -2654,7 +2660,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>489</v>
+        <v>309</v>
       </c>
       <c r="B87" t="s">
         <v>274</v>
@@ -2662,7 +2668,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B88" t="s">
         <v>274</v>
@@ -2670,23 +2676,23 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>489</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>274</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>490</v>
       </c>
       <c r="B90" t="s">
-        <v>91</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>91</v>
@@ -2694,7 +2700,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
         <v>91</v>
@@ -2702,7 +2708,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
         <v>91</v>
@@ -2710,7 +2716,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B94" t="s">
         <v>91</v>
@@ -2718,7 +2724,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B95" t="s">
         <v>91</v>
@@ -2726,7 +2732,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B96" t="s">
         <v>91</v>
@@ -2734,7 +2740,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
         <v>91</v>
@@ -2742,7 +2748,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B98" t="s">
         <v>91</v>
@@ -2750,7 +2756,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
         <v>91</v>
@@ -2758,7 +2764,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
         <v>91</v>
@@ -2766,7 +2772,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>91</v>
@@ -2774,7 +2780,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
         <v>91</v>
@@ -2782,7 +2788,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
         <v>91</v>
@@ -2790,7 +2796,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
         <v>91</v>
@@ -2798,7 +2804,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B105" t="s">
         <v>91</v>
@@ -2806,7 +2812,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B106" t="s">
         <v>91</v>
@@ -2814,7 +2820,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B107" t="s">
         <v>91</v>
@@ -2822,7 +2828,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
         <v>91</v>
@@ -2830,7 +2836,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B109" t="s">
         <v>91</v>
@@ -2838,7 +2844,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B110" t="s">
         <v>91</v>
@@ -2846,7 +2852,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B111" t="s">
         <v>91</v>
@@ -2854,7 +2860,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B112" t="s">
         <v>91</v>
@@ -2862,7 +2868,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B113" t="s">
         <v>91</v>
@@ -2870,7 +2876,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B114" t="s">
         <v>91</v>
@@ -2878,7 +2884,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B115" t="s">
         <v>91</v>
@@ -2886,7 +2892,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B116" t="s">
         <v>91</v>
@@ -2894,7 +2900,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>412</v>
+        <v>117</v>
       </c>
       <c r="B117" t="s">
         <v>91</v>
@@ -2902,7 +2908,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>413</v>
+        <v>118</v>
       </c>
       <c r="B118" t="s">
         <v>91</v>
@@ -2910,7 +2916,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B119" t="s">
         <v>91</v>
@@ -2918,7 +2924,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B120" t="s">
         <v>91</v>
@@ -2926,7 +2932,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>414</v>
       </c>
       <c r="B121" t="s">
         <v>91</v>
@@ -2934,7 +2940,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B122" t="s">
         <v>91</v>
@@ -2942,7 +2948,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>417</v>
+        <v>119</v>
       </c>
       <c r="B123" t="s">
         <v>91</v>
@@ -2950,7 +2956,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B124" t="s">
         <v>91</v>
@@ -2958,7 +2964,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B125" t="s">
         <v>91</v>
@@ -2966,7 +2972,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B126" t="s">
         <v>91</v>
@@ -2974,7 +2980,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="B127" t="s">
         <v>91</v>
@@ -2982,7 +2988,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>342</v>
+        <v>420</v>
       </c>
       <c r="B128" t="s">
         <v>91</v>
@@ -2990,7 +2996,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>343</v>
+        <v>120</v>
       </c>
       <c r="B129" t="s">
         <v>91</v>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B130" t="s">
         <v>91</v>
@@ -3006,7 +3012,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B131" t="s">
         <v>91</v>
@@ -3014,7 +3020,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B132" t="s">
         <v>91</v>
@@ -3022,7 +3028,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B133" t="s">
         <v>91</v>
@@ -3030,7 +3036,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B134" t="s">
         <v>91</v>
@@ -3038,7 +3044,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B135" t="s">
         <v>91</v>
@@ -3046,7 +3052,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B136" t="s">
         <v>91</v>
@@ -3054,7 +3060,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B137" t="s">
         <v>91</v>
@@ -3062,7 +3068,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B138" t="s">
         <v>91</v>
@@ -3070,7 +3076,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B139" t="s">
         <v>91</v>
@@ -3078,7 +3084,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B140" t="s">
         <v>91</v>
@@ -3086,7 +3092,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B141" t="s">
         <v>91</v>
@@ -3094,7 +3100,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B142" t="s">
         <v>91</v>
@@ -3102,7 +3108,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B143" t="s">
         <v>91</v>
@@ -3110,7 +3116,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B144" t="s">
         <v>91</v>
@@ -3118,7 +3124,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B145" t="s">
         <v>91</v>
@@ -3126,7 +3132,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B146" t="s">
         <v>91</v>
@@ -3134,7 +3140,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B147" t="s">
         <v>91</v>
@@ -3142,7 +3148,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B148" t="s">
         <v>91</v>
@@ -3150,7 +3156,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B149" t="s">
         <v>91</v>
@@ -3158,7 +3164,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B150" t="s">
         <v>91</v>
@@ -3166,7 +3172,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B151" t="s">
         <v>91</v>
@@ -3174,7 +3180,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B152" t="s">
         <v>91</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B153" t="s">
         <v>91</v>
@@ -3190,7 +3196,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B154" t="s">
         <v>91</v>
@@ -3198,7 +3204,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B155" t="s">
         <v>91</v>
@@ -3206,7 +3212,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B156" t="s">
         <v>91</v>
@@ -3214,7 +3220,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B157" t="s">
         <v>91</v>
@@ -3222,7 +3228,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>454</v>
+        <v>370</v>
       </c>
       <c r="B158" t="s">
         <v>91</v>
@@ -3230,7 +3236,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>455</v>
+        <v>371</v>
       </c>
       <c r="B159" t="s">
         <v>91</v>
@@ -3238,7 +3244,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B160" t="s">
         <v>91</v>
@@ -3246,7 +3252,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B161" t="s">
         <v>91</v>
@@ -3254,7 +3260,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B162" t="s">
         <v>91</v>
@@ -3262,7 +3268,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B163" t="s">
         <v>91</v>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>118</v>
+        <v>458</v>
       </c>
       <c r="B164" t="s">
         <v>91</v>
@@ -3278,7 +3284,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B165" t="s">
         <v>91</v>
@@ -3286,23 +3292,23 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>372</v>
+        <v>118</v>
       </c>
       <c r="B166" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>373</v>
+        <v>460</v>
       </c>
       <c r="B167" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B168" t="s">
         <v>122</v>
@@ -3310,7 +3316,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B169" t="s">
         <v>122</v>
@@ -3318,7 +3324,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B170" t="s">
         <v>122</v>
@@ -3326,7 +3332,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B171" t="s">
         <v>122</v>
@@ -3334,7 +3340,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B172" t="s">
         <v>122</v>
@@ -3342,7 +3348,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B173" t="s">
         <v>122</v>
@@ -3350,7 +3356,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B174" t="s">
         <v>122</v>
@@ -3358,7 +3364,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>121</v>
+        <v>379</v>
       </c>
       <c r="B175" t="s">
         <v>122</v>
@@ -3366,7 +3372,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>123</v>
+        <v>380</v>
       </c>
       <c r="B176" t="s">
         <v>122</v>
@@ -3374,15 +3380,15 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B177" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="2" t="s">
-        <v>125</v>
+      <c r="A178" t="s">
+        <v>123</v>
       </c>
       <c r="B178" t="s">
         <v>122</v>
@@ -3390,15 +3396,15 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B179" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>127</v>
+      <c r="A180" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B180" t="s">
         <v>122</v>
@@ -3406,7 +3412,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B181" t="s">
         <v>122</v>
@@ -3414,7 +3420,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B182" t="s">
         <v>122</v>
@@ -3422,7 +3428,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B183" t="s">
         <v>122</v>
@@ -3430,7 +3436,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B184" t="s">
         <v>122</v>
@@ -3438,7 +3444,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B185" t="s">
         <v>122</v>
@@ -3446,7 +3452,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B186" t="s">
         <v>122</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B187" t="s">
         <v>122</v>
@@ -3462,7 +3468,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B188" t="s">
         <v>122</v>
@@ -3470,7 +3476,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B189" t="s">
         <v>122</v>
@@ -3478,7 +3484,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B190" t="s">
         <v>122</v>
@@ -3486,7 +3492,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B191" t="s">
         <v>122</v>
@@ -3494,7 +3500,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B192" t="s">
         <v>122</v>
@@ -3502,7 +3508,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B193" t="s">
         <v>122</v>
@@ -3510,7 +3516,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B194" t="s">
         <v>122</v>
@@ -3518,7 +3524,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B195" t="s">
         <v>122</v>
@@ -3526,7 +3532,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B196" t="s">
         <v>122</v>
@@ -3534,7 +3540,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B197" t="s">
         <v>122</v>
@@ -3542,7 +3548,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B198" t="s">
         <v>122</v>
@@ -3550,7 +3556,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B199" t="s">
         <v>122</v>
@@ -3558,7 +3564,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B200" t="s">
         <v>122</v>
@@ -3566,7 +3572,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B201" t="s">
         <v>122</v>
@@ -3574,7 +3580,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B202" t="s">
         <v>122</v>
@@ -3582,7 +3588,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B203" t="s">
         <v>122</v>
@@ -3590,7 +3596,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B204" t="s">
         <v>122</v>
@@ -3598,7 +3604,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B205" t="s">
         <v>122</v>
@@ -3606,7 +3612,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B206" t="s">
         <v>122</v>
@@ -3614,7 +3620,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B207" t="s">
         <v>122</v>
@@ -3622,7 +3628,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B208" t="s">
         <v>122</v>
@@ -3630,7 +3636,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B209" t="s">
         <v>122</v>
@@ -3638,7 +3644,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B210" t="s">
         <v>122</v>
@@ -3646,7 +3652,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>373</v>
+        <v>156</v>
       </c>
       <c r="B211" t="s">
         <v>122</v>
@@ -3654,7 +3660,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B212" t="s">
         <v>122</v>
@@ -3662,7 +3668,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>159</v>
+        <v>373</v>
       </c>
       <c r="B213" t="s">
         <v>122</v>
@@ -3670,7 +3676,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B214" t="s">
         <v>122</v>
@@ -3678,7 +3684,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B215" t="s">
         <v>122</v>
@@ -3686,7 +3692,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B216" t="s">
         <v>122</v>
@@ -3694,7 +3700,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B217" t="s">
         <v>122</v>
@@ -3702,7 +3708,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B218" t="s">
         <v>122</v>
@@ -3710,7 +3716,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B219" t="s">
         <v>122</v>
@@ -3718,7 +3724,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B220" t="s">
         <v>122</v>
@@ -3726,7 +3732,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B221" t="s">
         <v>122</v>
@@ -3734,7 +3740,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B222" t="s">
         <v>122</v>
@@ -3742,7 +3748,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B223" t="s">
         <v>122</v>
@@ -3750,7 +3756,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B224" t="s">
         <v>122</v>
@@ -3758,7 +3764,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B225" t="s">
         <v>122</v>
@@ -3766,7 +3772,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B226" t="s">
         <v>122</v>
@@ -3774,7 +3780,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B227" t="s">
         <v>122</v>
@@ -3782,7 +3788,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>461</v>
+        <v>172</v>
       </c>
       <c r="B228" t="s">
         <v>122</v>
@@ -3790,7 +3796,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>462</v>
+        <v>173</v>
       </c>
       <c r="B229" t="s">
         <v>122</v>
@@ -3798,7 +3804,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B230" t="s">
         <v>122</v>
@@ -3806,7 +3812,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B231" t="s">
         <v>122</v>
@@ -3814,7 +3820,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B232" t="s">
         <v>122</v>
@@ -3822,7 +3828,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B233" t="s">
         <v>122</v>
@@ -3830,7 +3836,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B234" t="s">
         <v>122</v>
@@ -3838,7 +3844,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B235" t="s">
         <v>122</v>
@@ -3846,23 +3852,23 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>16</v>
+        <v>467</v>
       </c>
       <c r="B236" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>12</v>
+        <v>468</v>
       </c>
       <c r="B237" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B238" t="s">
         <v>13</v>
@@ -3870,7 +3876,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B239" t="s">
         <v>13</v>
@@ -3886,7 +3892,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B241" t="s">
         <v>13</v>
@@ -3894,7 +3900,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B242" t="s">
         <v>13</v>
@@ -3902,7 +3908,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B243" t="s">
         <v>13</v>
@@ -3910,7 +3916,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B244" t="s">
         <v>13</v>
@@ -3918,7 +3924,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B245" t="s">
         <v>13</v>
@@ -3926,7 +3932,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B246" t="s">
         <v>13</v>
@@ -3934,7 +3940,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B247" t="s">
         <v>13</v>
@@ -3942,7 +3948,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B248" t="s">
         <v>13</v>
@@ -3950,7 +3956,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>438</v>
+        <v>28</v>
       </c>
       <c r="B249" t="s">
         <v>13</v>
@@ -3958,7 +3964,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>439</v>
+        <v>36</v>
       </c>
       <c r="B250" t="s">
         <v>13</v>
@@ -3966,7 +3972,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B251" t="s">
         <v>13</v>
@@ -3974,7 +3980,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B252" t="s">
         <v>13</v>
@@ -3982,7 +3988,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B253" t="s">
         <v>13</v>
@@ -3990,7 +3996,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B254" t="s">
         <v>13</v>
@@ -3998,7 +4004,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B255" t="s">
         <v>13</v>
@@ -4006,7 +4012,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B256" t="s">
         <v>13</v>
@@ -4014,23 +4020,23 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>421</v>
+        <v>444</v>
       </c>
       <c r="B257" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>2</v>
+        <v>445</v>
       </c>
       <c r="B258" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>4</v>
+        <v>421</v>
       </c>
       <c r="B259" t="s">
         <v>3</v>
@@ -4038,7 +4044,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B260" t="s">
         <v>3</v>
@@ -4046,7 +4052,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B261" t="s">
         <v>3</v>
@@ -4054,7 +4060,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B262" t="s">
         <v>3</v>
@@ -4062,7 +4068,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B263" t="s">
         <v>3</v>
@@ -4070,7 +4076,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B264" t="s">
         <v>3</v>
@@ -4078,7 +4084,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B265" t="s">
         <v>3</v>
@@ -4086,7 +4092,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B266" t="s">
         <v>3</v>
@@ -4094,7 +4100,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B267" t="s">
         <v>3</v>
@@ -4102,7 +4108,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B268" t="s">
         <v>3</v>
@@ -4110,7 +4116,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B269" t="s">
         <v>3</v>
@@ -4118,7 +4124,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B270" t="s">
         <v>3</v>
@@ -4126,7 +4132,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B271" t="s">
         <v>3</v>
@@ -4134,7 +4140,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B272" t="s">
         <v>3</v>
@@ -4142,7 +4148,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B273" t="s">
         <v>3</v>
@@ -4150,7 +4156,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B274" t="s">
         <v>3</v>
@@ -4158,7 +4164,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B275" t="s">
         <v>3</v>
@@ -4166,7 +4172,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B276" t="s">
         <v>3</v>
@@ -4174,7 +4180,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B277" t="s">
         <v>3</v>
@@ -4182,7 +4188,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B278" t="s">
         <v>3</v>
@@ -4190,7 +4196,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B279" t="s">
         <v>3</v>
@@ -4198,7 +4204,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>422</v>
+        <v>34</v>
       </c>
       <c r="B280" t="s">
         <v>3</v>
@@ -4206,7 +4212,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>423</v>
+        <v>29</v>
       </c>
       <c r="B281" t="s">
         <v>3</v>
@@ -4214,7 +4220,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B282" t="s">
         <v>3</v>
@@ -4222,7 +4228,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B283" t="s">
         <v>3</v>
@@ -4230,7 +4236,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B284" t="s">
         <v>3</v>
@@ -4238,7 +4244,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B285" t="s">
         <v>3</v>
@@ -4246,7 +4252,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B286" t="s">
         <v>3</v>
@@ -4254,7 +4260,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B287" t="s">
         <v>3</v>
@@ -4262,23 +4268,23 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>312</v>
+        <v>428</v>
       </c>
       <c r="B288" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>313</v>
+        <v>429</v>
       </c>
       <c r="B289" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B290" t="s">
         <v>50</v>
@@ -4286,7 +4292,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>411</v>
+        <v>313</v>
       </c>
       <c r="B291" t="s">
         <v>50</v>
@@ -4294,7 +4300,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>51</v>
+        <v>314</v>
       </c>
       <c r="B292" t="s">
         <v>50</v>
@@ -4302,7 +4308,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>52</v>
+        <v>411</v>
       </c>
       <c r="B293" t="s">
         <v>50</v>
@@ -4310,7 +4316,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B294" t="s">
         <v>50</v>
@@ -4318,7 +4324,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B295" t="s">
         <v>50</v>
@@ -4326,7 +4332,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B296" t="s">
         <v>50</v>
@@ -4334,7 +4340,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B297" t="s">
         <v>50</v>
@@ -4342,7 +4348,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B298" t="s">
         <v>50</v>
@@ -4350,7 +4356,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B299" t="s">
         <v>50</v>
@@ -4358,7 +4364,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B300" t="s">
         <v>50</v>
@@ -4366,7 +4372,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B301" t="s">
         <v>50</v>
@@ -4374,7 +4380,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B302" t="s">
         <v>50</v>
@@ -4382,7 +4388,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B303" t="s">
         <v>50</v>
@@ -4390,7 +4396,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B304" t="s">
         <v>50</v>
@@ -4398,7 +4404,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B305" t="s">
         <v>50</v>
@@ -4406,7 +4412,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B306" t="s">
         <v>50</v>
@@ -4414,7 +4420,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B307" t="s">
         <v>50</v>
@@ -4422,7 +4428,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B308" t="s">
         <v>50</v>
@@ -4430,7 +4436,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B309" t="s">
         <v>50</v>
@@ -4438,7 +4444,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B310" t="s">
         <v>50</v>
@@ -4446,7 +4452,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B311" t="s">
         <v>50</v>
@@ -4454,7 +4460,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B312" t="s">
         <v>50</v>
@@ -4462,7 +4468,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B313" t="s">
         <v>50</v>
@@ -4470,7 +4476,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B314" t="s">
         <v>50</v>
@@ -4478,7 +4484,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B315" t="s">
         <v>50</v>
@@ -4486,7 +4492,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B316" t="s">
         <v>50</v>
@@ -4494,7 +4500,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B317" t="s">
         <v>50</v>
@@ -4502,7 +4508,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B318" t="s">
         <v>50</v>
@@ -4510,7 +4516,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B319" t="s">
         <v>50</v>
@@ -4518,7 +4524,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B320" t="s">
         <v>50</v>
@@ -4526,7 +4532,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B321" t="s">
         <v>50</v>
@@ -4534,7 +4540,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B322" t="s">
         <v>50</v>
@@ -4542,7 +4548,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B323" t="s">
         <v>50</v>
@@ -4550,7 +4556,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B324" t="s">
         <v>50</v>
@@ -4558,7 +4564,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B325" t="s">
         <v>50</v>
@@ -4566,7 +4572,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B326" t="s">
         <v>50</v>
@@ -4574,7 +4580,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B327" t="s">
         <v>50</v>
@@ -4582,7 +4588,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B328" t="s">
         <v>50</v>
@@ -4590,7 +4596,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B329" t="s">
         <v>50</v>
@@ -4598,7 +4604,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B330" t="s">
         <v>50</v>
@@ -4606,7 +4612,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>315</v>
+        <v>88</v>
       </c>
       <c r="B331" t="s">
         <v>50</v>
@@ -4614,7 +4620,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>316</v>
+        <v>89</v>
       </c>
       <c r="B332" t="s">
         <v>50</v>
@@ -4622,7 +4628,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B333" t="s">
         <v>50</v>
@@ -4630,7 +4636,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B334" t="s">
         <v>50</v>
@@ -4638,7 +4644,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B335" t="s">
         <v>50</v>
@@ -4646,7 +4652,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B336" t="s">
         <v>50</v>
@@ -4654,7 +4660,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B337" t="s">
         <v>50</v>
@@ -4662,7 +4668,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B338" t="s">
         <v>50</v>
@@ -4670,7 +4676,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B339" t="s">
         <v>50</v>
@@ -4678,7 +4684,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B340" t="s">
         <v>50</v>
@@ -4686,7 +4692,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B341" t="s">
         <v>50</v>
@@ -4694,7 +4700,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B342" t="s">
         <v>50</v>
@@ -4702,7 +4708,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B343" t="s">
         <v>50</v>
@@ -4710,7 +4716,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B344" t="s">
         <v>50</v>
@@ -4718,7 +4724,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B345" t="s">
         <v>50</v>
@@ -4726,7 +4732,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B346" t="s">
         <v>50</v>
@@ -4734,7 +4740,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B347" t="s">
         <v>50</v>
@@ -4742,7 +4748,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B348" t="s">
         <v>50</v>
@@ -4750,7 +4756,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B349" t="s">
         <v>50</v>
@@ -4758,7 +4764,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B350" t="s">
         <v>50</v>
@@ -4766,7 +4772,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B351" t="s">
         <v>50</v>
@@ -4774,7 +4780,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B352" t="s">
         <v>50</v>
@@ -4782,7 +4788,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B353" t="s">
         <v>50</v>
@@ -4790,7 +4796,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B354" t="s">
         <v>50</v>
@@ -4798,7 +4804,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B355" t="s">
         <v>50</v>
@@ -4806,7 +4812,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B356" t="s">
         <v>50</v>
@@ -4814,7 +4820,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B357" t="s">
         <v>50</v>
@@ -4822,7 +4828,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>446</v>
+        <v>340</v>
       </c>
       <c r="B358" t="s">
         <v>50</v>
@@ -4830,7 +4836,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>447</v>
+        <v>341</v>
       </c>
       <c r="B359" t="s">
         <v>50</v>
@@ -4838,7 +4844,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B360" t="s">
         <v>50</v>
@@ -4846,7 +4852,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B361" t="s">
         <v>50</v>
@@ -4854,7 +4860,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B362" t="s">
         <v>50</v>
@@ -4862,7 +4868,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B363" t="s">
         <v>50</v>
@@ -4870,7 +4876,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B364" t="s">
         <v>50</v>
@@ -4878,7 +4884,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B365" t="s">
         <v>50</v>
@@ -4886,23 +4892,23 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>174</v>
+        <v>452</v>
       </c>
       <c r="B366" t="s">
-        <v>175</v>
+        <v>50</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>176</v>
+        <v>453</v>
       </c>
       <c r="B367" t="s">
-        <v>175</v>
+        <v>50</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B368" t="s">
         <v>175</v>
@@ -4910,7 +4916,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B369" t="s">
         <v>175</v>
@@ -4918,7 +4924,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B370" t="s">
         <v>175</v>
@@ -4926,7 +4932,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B371" t="s">
         <v>175</v>
@@ -4934,7 +4940,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B372" t="s">
         <v>175</v>
@@ -4942,7 +4948,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B373" t="s">
         <v>175</v>
@@ -4950,7 +4956,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B374" t="s">
         <v>175</v>
@@ -4958,7 +4964,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B375" t="s">
         <v>175</v>
@@ -4966,7 +4972,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B376" t="s">
         <v>175</v>
@@ -4974,7 +4980,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B377" t="s">
         <v>175</v>
@@ -4982,7 +4988,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B378" t="s">
         <v>175</v>
@@ -4990,7 +4996,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B379" t="s">
         <v>175</v>
@@ -4998,7 +5004,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B380" t="s">
         <v>175</v>
@@ -5006,7 +5012,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B381" t="s">
         <v>175</v>
@@ -5014,7 +5020,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B382" t="s">
         <v>175</v>
@@ -5022,7 +5028,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B383" t="s">
         <v>175</v>
@@ -5030,7 +5036,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B384" t="s">
         <v>175</v>
@@ -5038,7 +5044,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B385" t="s">
         <v>175</v>
@@ -5046,7 +5052,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B386" t="s">
         <v>175</v>
@@ -5054,7 +5060,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B387" t="s">
         <v>175</v>
@@ -5062,7 +5068,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B388" t="s">
         <v>175</v>
@@ -5070,7 +5076,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B389" t="s">
         <v>175</v>
@@ -5078,7 +5084,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B390" t="s">
         <v>175</v>
@@ -5086,7 +5092,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B391" t="s">
         <v>175</v>
@@ -5094,7 +5100,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B392" t="s">
         <v>175</v>
@@ -5102,7 +5108,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B393" t="s">
         <v>175</v>
@@ -5110,7 +5116,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>381</v>
+        <v>201</v>
       </c>
       <c r="B394" t="s">
         <v>175</v>
@@ -5118,7 +5124,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B395" t="s">
         <v>175</v>
@@ -5126,7 +5132,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>204</v>
+        <v>381</v>
       </c>
       <c r="B396" t="s">
         <v>175</v>
@@ -5134,7 +5140,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B397" t="s">
         <v>175</v>
@@ -5142,7 +5148,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B398" t="s">
         <v>175</v>
@@ -5150,7 +5156,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B399" t="s">
         <v>175</v>
@@ -5158,7 +5164,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B400" t="s">
         <v>175</v>
@@ -5166,7 +5172,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B401" t="s">
         <v>175</v>
@@ -5174,7 +5180,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
-        <v>382</v>
+        <v>208</v>
       </c>
       <c r="B402" t="s">
         <v>175</v>
@@ -5182,7 +5188,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>383</v>
+        <v>209</v>
       </c>
       <c r="B403" t="s">
         <v>175</v>
@@ -5190,7 +5196,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B404" t="s">
         <v>175</v>
@@ -5198,7 +5204,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B405" t="s">
         <v>175</v>
@@ -5206,7 +5212,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B406" t="s">
         <v>175</v>
@@ -5214,7 +5220,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B407" t="s">
         <v>175</v>
@@ -5222,7 +5228,7 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B408" t="s">
         <v>175</v>
@@ -5230,7 +5236,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B409" t="s">
         <v>175</v>
@@ -5238,7 +5244,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B410" t="s">
         <v>175</v>
@@ -5246,7 +5252,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B411" t="s">
         <v>175</v>
@@ -5254,7 +5260,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B412" t="s">
         <v>175</v>
@@ -5262,7 +5268,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>178</v>
+        <v>391</v>
       </c>
       <c r="B413" t="s">
         <v>175</v>
@@ -5270,7 +5276,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B414" t="s">
         <v>175</v>
@@ -5278,7 +5284,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>394</v>
+        <v>178</v>
       </c>
       <c r="B415" t="s">
         <v>175</v>
@@ -5286,7 +5292,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B416" t="s">
         <v>175</v>
@@ -5294,7 +5300,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
-        <v>469</v>
+        <v>394</v>
       </c>
       <c r="B417" t="s">
         <v>175</v>
@@ -5302,7 +5308,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>178</v>
+        <v>395</v>
       </c>
       <c r="B418" t="s">
         <v>175</v>
@@ -5310,7 +5316,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B419" t="s">
         <v>175</v>
@@ -5318,7 +5324,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
-        <v>471</v>
+        <v>178</v>
       </c>
       <c r="B420" t="s">
         <v>175</v>
@@ -5326,7 +5332,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B421" t="s">
         <v>175</v>
@@ -5334,7 +5340,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B422" t="s">
         <v>175</v>
@@ -5342,7 +5348,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B423" t="s">
         <v>175</v>
@@ -5350,7 +5356,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B424" t="s">
         <v>175</v>
@@ -5358,23 +5364,23 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
-        <v>210</v>
+        <v>474</v>
       </c>
       <c r="B425" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
-        <v>212</v>
+        <v>475</v>
       </c>
       <c r="B426" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B427" t="s">
         <v>211</v>
@@ -5382,7 +5388,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B428" t="s">
         <v>211</v>
@@ -5390,7 +5396,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B429" t="s">
         <v>211</v>
@@ -5398,7 +5404,7 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B430" t="s">
         <v>211</v>
@@ -5406,7 +5412,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B431" t="s">
         <v>211</v>
@@ -5414,7 +5420,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B432" t="s">
         <v>211</v>
@@ -5422,7 +5428,7 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B433" t="s">
         <v>211</v>
@@ -5430,7 +5436,7 @@
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B434" t="s">
         <v>211</v>
@@ -5438,7 +5444,7 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B435" t="s">
         <v>211</v>
@@ -5446,7 +5452,7 @@
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B436" t="s">
         <v>211</v>
@@ -5454,7 +5460,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B437" t="s">
         <v>211</v>
@@ -5462,7 +5468,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B438" t="s">
         <v>211</v>
@@ -5470,7 +5476,7 @@
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B439" t="s">
         <v>211</v>
@@ -5478,7 +5484,7 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B440" t="s">
         <v>211</v>
@@ -5486,7 +5492,7 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B441" t="s">
         <v>211</v>
@@ -5494,7 +5500,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B442" t="s">
         <v>211</v>
@@ -5502,7 +5508,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B443" t="s">
         <v>211</v>
@@ -5510,7 +5516,7 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B444" t="s">
         <v>211</v>
@@ -5518,7 +5524,7 @@
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B445" t="s">
         <v>211</v>
@@ -5526,7 +5532,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B446" t="s">
         <v>211</v>
@@ -5534,7 +5540,7 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B447" t="s">
         <v>211</v>
@@ -5542,7 +5548,7 @@
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B448" t="s">
         <v>211</v>
@@ -5550,7 +5556,7 @@
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B449" t="s">
         <v>211</v>
@@ -5558,7 +5564,7 @@
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B450" t="s">
         <v>211</v>
@@ -5566,7 +5572,7 @@
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B451" t="s">
         <v>211</v>
@@ -5574,7 +5580,7 @@
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B452" t="s">
         <v>211</v>
@@ -5582,7 +5588,7 @@
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B453" t="s">
         <v>211</v>
@@ -5590,7 +5596,7 @@
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B454" t="s">
         <v>211</v>
@@ -5598,7 +5604,7 @@
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B455" t="s">
         <v>211</v>
@@ -5606,7 +5612,7 @@
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B456" t="s">
         <v>211</v>
@@ -5614,7 +5620,7 @@
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B457" t="s">
         <v>211</v>
@@ -5622,7 +5628,7 @@
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B458" t="s">
         <v>211</v>
@@ -5630,7 +5636,7 @@
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B459" t="s">
         <v>211</v>
@@ -5638,7 +5644,7 @@
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B460" t="s">
         <v>211</v>
@@ -5646,7 +5652,7 @@
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B461" t="s">
         <v>211</v>
@@ -5654,7 +5660,7 @@
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B462" t="s">
         <v>211</v>
@@ -5662,7 +5668,7 @@
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B463" t="s">
         <v>211</v>
@@ -5670,7 +5676,7 @@
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B464" t="s">
         <v>211</v>
@@ -5678,7 +5684,7 @@
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B465" t="s">
         <v>211</v>
@@ -5686,7 +5692,7 @@
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B466" t="s">
         <v>211</v>
@@ -5694,7 +5700,7 @@
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B467" t="s">
         <v>211</v>
@@ -5702,7 +5708,7 @@
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B468" t="s">
         <v>211</v>
@@ -5710,7 +5716,7 @@
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B469" t="s">
         <v>211</v>
@@ -5718,7 +5724,7 @@
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B470" t="s">
         <v>211</v>
@@ -5726,7 +5732,7 @@
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B471" t="s">
         <v>211</v>
@@ -5734,7 +5740,7 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B472" t="s">
         <v>211</v>
@@ -5742,7 +5748,7 @@
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B473" t="s">
         <v>211</v>
@@ -5750,7 +5756,7 @@
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B474" t="s">
         <v>211</v>
@@ -5758,7 +5764,7 @@
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B475" t="s">
         <v>211</v>
@@ -5766,7 +5772,7 @@
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B476" t="s">
         <v>211</v>
@@ -5774,7 +5780,7 @@
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B477" t="s">
         <v>211</v>
@@ -5782,7 +5788,7 @@
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B478" t="s">
         <v>211</v>
@@ -5790,7 +5796,7 @@
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B479" t="s">
         <v>211</v>
@@ -5798,7 +5804,7 @@
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B480" t="s">
         <v>211</v>
@@ -5806,7 +5812,7 @@
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B481" t="s">
         <v>211</v>
@@ -5814,7 +5820,7 @@
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B482" t="s">
         <v>211</v>
@@ -5822,7 +5828,7 @@
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B483" t="s">
         <v>211</v>
@@ -5830,7 +5836,7 @@
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B484" t="s">
         <v>211</v>
@@ -5838,7 +5844,7 @@
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B485" t="s">
         <v>211</v>
@@ -5846,7 +5852,7 @@
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B486" t="s">
         <v>211</v>
@@ -5854,7 +5860,7 @@
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
-        <v>476</v>
+        <v>271</v>
       </c>
       <c r="B487" t="s">
         <v>211</v>
@@ -5862,7 +5868,7 @@
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
-        <v>477</v>
+        <v>272</v>
       </c>
       <c r="B488" t="s">
         <v>211</v>
@@ -5870,7 +5876,7 @@
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B489" t="s">
         <v>211</v>
@@ -5878,7 +5884,7 @@
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B490" t="s">
         <v>211</v>
@@ -5886,7 +5892,7 @@
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B491" t="s">
         <v>211</v>
@@ -5894,7 +5900,7 @@
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B492" t="s">
         <v>211</v>
@@ -5902,7 +5908,7 @@
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B493" t="s">
         <v>211</v>
@@ -5910,7 +5916,7 @@
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B494" t="s">
         <v>211</v>
@@ -5918,31 +5924,31 @@
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
-        <v>37</v>
+        <v>482</v>
       </c>
       <c r="B495" t="s">
-        <v>38</v>
+        <v>211</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
-        <v>39</v>
+        <v>483</v>
       </c>
       <c r="B496" t="s">
-        <v>38</v>
+        <v>211</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B497" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A498" s="1" t="s">
-        <v>41</v>
+      <c r="A498" t="s">
+        <v>39</v>
       </c>
       <c r="B498" t="s">
         <v>38</v>
@@ -5950,31 +5956,31 @@
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B499" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A500" t="s">
-        <v>43</v>
+      <c r="A500" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B500" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A501" s="1" t="s">
-        <v>44</v>
+      <c r="A501" t="s">
+        <v>42</v>
       </c>
       <c r="B501" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A502" s="1" t="s">
-        <v>45</v>
+      <c r="A502" t="s">
+        <v>43</v>
       </c>
       <c r="B502" t="s">
         <v>38</v>
@@ -5982,7 +5988,7 @@
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A503" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B503" t="s">
         <v>38</v>
@@ -5990,23 +5996,23 @@
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A504" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B504" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A505" t="s">
-        <v>48</v>
+      <c r="A505" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B505" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A506" t="s">
-        <v>49</v>
+      <c r="A506" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B506" t="s">
         <v>38</v>
@@ -6014,7 +6020,7 @@
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
-        <v>430</v>
+        <v>48</v>
       </c>
       <c r="B507" t="s">
         <v>38</v>
@@ -6022,7 +6028,7 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
-        <v>431</v>
+        <v>49</v>
       </c>
       <c r="B508" t="s">
         <v>38</v>
@@ -6030,7 +6036,7 @@
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B509" t="s">
         <v>38</v>
@@ -6038,7 +6044,7 @@
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B510" t="s">
         <v>38</v>
@@ -6046,7 +6052,7 @@
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B511" t="s">
         <v>38</v>
@@ -6054,7 +6060,7 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B512" t="s">
         <v>38</v>
@@ -6062,7 +6068,7 @@
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B513" t="s">
         <v>38</v>
@@ -6070,15 +6076,31 @@
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B514" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>436</v>
+      </c>
+      <c r="B515" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>437</v>
+      </c>
+      <c r="B516" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B514">
-    <sortCondition ref="B2:B514"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B516">
+    <sortCondition ref="B2:B516"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
key-value pairing on certain input message to intent
</commit_message>
<xml_diff>
--- a/app/algorithm/database/data.xlsx
+++ b/app/algorithm/database/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\IAI\app\algorithm\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9573CFB2-26B5-436A-88AB-455827521017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B64B13-035C-4E23-8E25-A505B1D6FCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11076" yWindow="132" windowWidth="11796" windowHeight="11880" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F56ACAE5-2C64-4881-A454-41EAB5000D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -3310,7 +3310,7 @@
   <dimension ref="A1:B938"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
-      <selection activeCell="B397" sqref="B396:B397"/>
+      <selection activeCell="A390" sqref="A390:XFD393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>